<commit_message>
Update to add non blocking timer
This update is designed to remove the need for a blocking delay in the timer. The ReportDelay variable holds the minimum time (500ms) between lcd refreshes. When the current time minus the last reporting time exceeds this delay lcdReport is called. This function clears the lcd, and prints the last updated values for voltage and steinhart. Credit to user romankaelin for highlighting the limitations of using a blocking delay in the previous iteration of the code.
</commit_message>
<xml_diff>
--- a/Steinhart Working.xlsx
+++ b/Steinhart Working.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roaster\OneDrive\8.0 - Projects\8.53 - LM Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roaster\Dropbox\LaMarzoccoTempSensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{5B116CC5-3041-4036-AB1C-896E08879B9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{835D3194-C548-4DBF-A73B-7F52712EFF14}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE8BA65-79BB-47CF-9515-297042C8EDCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1367DDE6-AAB7-41C9-B995-9B800C4D1040}"/>
+    <workbookView minimized="1" xWindow="7635" yWindow="1605" windowWidth="20205" windowHeight="12330" xr2:uid="{1367DDE6-AAB7-41C9-B995-9B800C4D1040}"/>
   </bookViews>
   <sheets>
     <sheet name="SteinHart" sheetId="2" r:id="rId1"/>
@@ -200,7 +200,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -260,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -270,19 +270,19 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.0"/>
+      <numFmt numFmtId="165" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.0"/>
+      <numFmt numFmtId="165" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.0"/>
+      <numFmt numFmtId="165" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.0"/>
+      <numFmt numFmtId="165" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3279,6 +3279,2303 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4E56-4707-A165-D86010BFE653}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'LM Thermistor Data'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nominal (kΩ)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.29860047081743646"/>
+                  <c:y val="-4.8237506821548384E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'LM Thermistor Data'!$A$4:$A$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'LM Thermistor Data'!$C$4:$C$94</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>98.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89.29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81.19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73.91</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>67.36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64.34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>61.47</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58.74</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>56.15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>53.68</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>51.34</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49.12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44.99</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43.08</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41.25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39.520000000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>37.86</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>36.29</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>34.79</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33.46</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30.7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29.46</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.27</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>27.14</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>26.06</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>25.04</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24.05</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>23.11</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>22.22</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>21.36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20.54</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19.75</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>18.29</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>17.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4E56-4707-A165-D86010BFE653}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'LM Thermistor Data'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Maximum (kΩ)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'LM Thermistor Data'!$A$4:$A$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'LM Thermistor Data'!$D$4:$D$94</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>107.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.72</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88.68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84.52</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80.58</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>76.84</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>73.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>69.94</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>66.760000000000005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>63.74</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60.87</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>58.15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>55.56</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>53.11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50.78</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>48.56</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>46.45</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44.45</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42.54</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40.72</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37.35</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>35.79</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>32.880000000000003</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>31.52</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30.23</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>27.82</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>26.6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>25.63</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>24.61</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>23.64</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>22.71</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>21.82</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>20.97</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>20.16</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.38</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>18.64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4E56-4707-A165-D86010BFE653}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'LM Thermistor Data'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calc inverse (kΩ)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'LM Thermistor Data'!$A$4:$A$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'LM Thermistor Data'!$E$4:$E$94</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>99.582270328313996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94.779040718925117</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.238772625327812</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.945483120669479</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81.884251717102387</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78.041143973079087</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74.403140992000417</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.958074328207161</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>67.694565858430309</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64.601972215079783</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>61.67033341251603</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58.890325329056516</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>56.253215736222614</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>53.750823592894207</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>51.375481345866092</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49.12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46.977636740948192</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44.942064911458687</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43.007346158725973</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41.167904585271266</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39.418502749545794</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>37.754219374981041</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>36.17042863766072</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>34.66278091325686</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33.227184873453368</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>31.859790830846752</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30.556975239338175</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29.315326264388084</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.131630344239493</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>27.002859669396798</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>25.926160513313469</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>24.898842352441051</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>23.918367718567566</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>22.982342730756155</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>22.088508258224447</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>21.234731669206404</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20.418999124244262</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19.639408375489705</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>18.894162036475624</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>18.181561289474249</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>16.847959210269341</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>16.224001985503335</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15.626768588874473</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>15.054971962663389</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14.507393494821022</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>13.982879051635352</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>13.480335258591063</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>12.99872601279305</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>12.537069211510973</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>12.094433682497804</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>11.669936302749521</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>11.262739293310997</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10.872047678600996</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>10.49710689953303</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>10.137200570453418</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9.791648370606854</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9.4598040614795558</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9.1410536219622198</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>8.8348134938245941</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>8.5405289305032728</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>8.2576724426774888</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>7.9857423345469378</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7.7242613251332353</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>7.4727752493058999</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>7.2308518335857306</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.9980795421054358</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.7740664884122275</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.5584394090796243</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.350842695359586</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6.1509374793507225</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.9584007713870859</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.7729246455640784</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5.594215470516378</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.4219931827471273</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5.2559905999796763</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.095952772163459</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.941636367915299</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4.7928090943168487</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.6492491481190825</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.5107446965266114</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4.3770933858476546</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.2481018764019902</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.1235854021779144</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.0033673538221439</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.8872788836328285</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3.7751585313070586</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.6668518692698298</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.5622111664821596</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.4610950696925795</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.3633683011580624</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4E56-4707-A165-D86010BFE653}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1364495551"/>
+        <c:axId val="1393247695"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1364495551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1393247695"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1393247695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1364495551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'LM Thermistor Data'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minimum (kΩ)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'LM Thermistor Data'!$A$4:$A$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'LM Thermistor Data'!$B$4:$B$94</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>89.61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85.47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.540000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77.819999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70.930000000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>67.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64.739999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.87</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56.56</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>51.76</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49.53</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>47.42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43.49</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41.66</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39.92</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>38.270000000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>36.69</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>35.18</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33.75</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>32.380000000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>31.08</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>29.83</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28.64</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.51</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>26.43</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>25.39</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>24.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>23.46</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>22.55</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>21.69</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20.86</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>20.07</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>19.32</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>17.239999999999998</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>16.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EEE1-48F6-A816-6A8CF8C02ED8}"/>
             </c:ext>
           </c:extLst>
@@ -5154,6 +7451,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6741,6 +9078,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6913,6 +9766,44 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>467591</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>138546</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C79AF1F2-C311-4CAA-B7EA-8EBD92F39E42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -7358,8 +10249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AEF1D6-D6C3-45BA-9019-800874F1635E}">
   <dimension ref="A1:P153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="R77" sqref="R77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12561,7 +15452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ACA640-A789-4850-90AD-863774E615AB}">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>

</xml_diff>